<commit_message>
Fix excel + diagnosis
Repair of the Excel connection file and building a logic for diagnosis
</commit_message>
<xml_diff>
--- a/LoginInfo.xlsx
+++ b/LoginInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65b3116eb161f8cf/מסמכים/GitHub/QA-project/QA-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABDACC1048EBA11F51C65BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09356A12-70E9-456B-A6D9-BDC8FB326177}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF21302B-D14F-45C7-AD9E-1BA625DFE3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26475" yWindow="0" windowWidth="25125" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26895" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,24 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>yam</t>
+  </si>
+  <si>
+    <t>Yambit12</t>
+  </si>
+  <si>
+    <t>sjhfdasfhn</t>
+  </si>
+  <si>
+    <t>Y@123456</t>
+  </si>
+  <si>
+    <t>yambit33</t>
+  </si>
+  <si>
+    <t>fafasf</t>
   </si>
 </sst>
 </file>
@@ -405,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901EC5C4-B4DE-469B-A068-8E5576BCED1C}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -431,6 +449,34 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update and system comments
Termination of conditions regarding diseases according to the patient's blood tests
Plus system notes for better understanding
</commit_message>
<xml_diff>
--- a/LoginInfo.xlsx
+++ b/LoginInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ישראל\Documents\GitHub\QA-projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3418CE1B-72AF-499E-9A1F-E209527D3514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81884E16-9881-4609-8919-6973709FE1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="11208" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>i@123456</t>
+  </si>
+  <si>
+    <t>esti</t>
+  </si>
+  <si>
+    <t>esti19</t>
+  </si>
+  <si>
+    <t>ighfhgd</t>
+  </si>
+  <si>
+    <t>e@123456</t>
   </si>
 </sst>
 </file>
@@ -435,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901EC5C4-B4DE-469B-A068-8E5576BCED1C}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -503,6 +515,20 @@
       </c>
       <c r="D4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>